<commit_message>
Final code with comments indentation
</commit_message>
<xml_diff>
--- a/src/test/resources/Data.xlsx
+++ b/src/test/resources/Data.xlsx
@@ -22,7 +22,7 @@
     <t>Precision</t>
   </si>
   <si>
-    <t>Ajmer</t>
+    <t>Chennai</t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +385,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>